<commit_message>
Update to manuscript draft
- reorganized methods section
</commit_message>
<xml_diff>
--- a/report/drafting/2_27_2024/Figures/Table1_Shasta.xlsx
+++ b/report/drafting/2_27_2024/Figures/Table1_Shasta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattc\Documents\DL-reservoir-modeling\report\drafting\2_27_2024\Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419E1F38-A509-4A94-9869-A23C4CEB3B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609A8869-638F-4B4E-B59A-DD8503445B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Model 1</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Model 3</t>
   </si>
   <si>
-    <t>Model 1 (with storage)</t>
-  </si>
-  <si>
     <t>MC-LSTM</t>
   </si>
   <si>
@@ -58,6 +55,24 @@
   </si>
   <si>
     <t>Random Forest</t>
+  </si>
+  <si>
+    <t>Storage Inputted</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Model 1*</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linear* </t>
+  </si>
+  <si>
+    <t>Random Forest*</t>
   </si>
 </sst>
 </file>
@@ -121,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -135,6 +150,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,171 +431,228 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E9"/>
+      <selection activeCell="B2" sqref="B2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="25.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.3046875" customWidth="1"/>
-    <col min="4" max="4" width="22.15234375" customWidth="1"/>
-    <col min="5" max="5" width="16.921875" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="16.4609375" customWidth="1"/>
+    <col min="4" max="4" width="18.3046875" customWidth="1"/>
+    <col min="5" max="5" width="22.15234375" customWidth="1"/>
+    <col min="6" max="6" width="16.921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2">
         <v>0.73</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0.69</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>0.43</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
         <v>0.74</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>0.7</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>0.44</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4">
         <v>0.59</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>0.6</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>0.52</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2">
         <v>0.82</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>0.75</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>0.65</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
         <v>0.38</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>0.44</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>0.11</v>
       </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.42</v>
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D8" s="2">
-        <v>0.43</v>
+        <v>0.4</v>
       </c>
       <c r="E8" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+        <v>0.4</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.69</v>
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D9" s="2">
         <v>0.64</v>
       </c>
       <c r="E9" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.69</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="F11" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>